<commit_message>
more ch 6; average response scores by parameter
</commit_message>
<xml_diff>
--- a/average_precision/MAP-NS14-VS-NS50-all_features.xlsx
+++ b/average_precision/MAP-NS14-VS-NS50-all_features.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leviking/Documents/dissertation/SAILS/average_precision/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B30C9AF3-5D26-EB43-9326-5B39E7684967}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE1E4C6-9BCA-7C4F-B982-3CB377500449}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="14000" xr2:uid="{D73CB46D-A587-524B-B81B-789A60694153}"/>
+    <workbookView xWindow="860" yWindow="1440" windowWidth="24640" windowHeight="14000" xr2:uid="{D73CB46D-A587-524B-B81B-789A60694153}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="46">
   <si>
     <t>Total</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>N14 Core</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>diff</t>
   </si>
 </sst>
 </file>
@@ -526,15 +535,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1E68F4-9492-C047-9F81-416124BA915C}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>42</v>
       </c>
@@ -542,7 +551,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>40</v>
       </c>
@@ -573,8 +582,17 @@
       <c r="K2" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -608,8 +626,20 @@
       <c r="K3" s="1">
         <v>0.83065629949757247</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M3" s="1">
+        <f>MIN(B3:K10)</f>
+        <v>0.62867409822009668</v>
+      </c>
+      <c r="N3" s="1">
+        <f>MAX(B3:K10)</f>
+        <v>0.86534581767575869</v>
+      </c>
+      <c r="O3">
+        <f>ABS(M3-N3)</f>
+        <v>0.23667171945566201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -644,7 +674,7 @@
         <v>0.7011659706153639</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -679,7 +709,7 @@
         <v>0.62867409822009668</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -714,7 +744,7 @@
         <v>0.70423291416545941</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -749,7 +779,7 @@
         <v>0.73609799805656217</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -784,7 +814,7 @@
         <v>0.71888496165980709</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -819,7 +849,7 @@
         <v>0.7214459505622145</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -854,7 +884,7 @@
         <v>0.72016545611101113</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>35</v>
       </c>
@@ -862,7 +892,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -893,8 +923,17 @@
       <c r="K17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -928,8 +967,20 @@
       <c r="K18" s="1">
         <v>0.86767923802057234</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M18" s="1">
+        <f>MIN(B18:K25)</f>
+        <v>0.78667595283400127</v>
+      </c>
+      <c r="N18" s="1">
+        <f>MAX(B18:K25)</f>
+        <v>0.90000106100353749</v>
+      </c>
+      <c r="O18">
+        <f>ABS(M18-N18)</f>
+        <v>0.11332510816953623</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -964,7 +1015,7 @@
         <v>0.8382395004463431</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -999,7 +1050,7 @@
         <v>0.83265992191606986</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1085,7 @@
         <v>0.79757567831266596</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -1069,7 +1120,7 @@
         <v>0.89481009527599042</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1104,7 +1155,7 @@
         <v>0.8457680642829829</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1139,7 +1190,7 @@
         <v>0.84661770930567337</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1174,7 +1225,7 @@
         <v>0.84619288679432847</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>28</v>
       </c>
@@ -1182,7 +1233,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>26</v>
       </c>
@@ -1213,8 +1264,17 @@
       <c r="K29" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -1248,8 +1308,20 @@
       <c r="K30" s="1">
         <v>0.86358946827143401</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M30" s="1">
+        <f>MIN(B30:K37)</f>
+        <v>0.67945786918343476</v>
+      </c>
+      <c r="N30" s="1">
+        <f>MAX(B30:K37)</f>
+        <v>0.88668870883127349</v>
+      </c>
+      <c r="O30">
+        <f>ABS(M30-N30)</f>
+        <v>0.20723083964783873</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1283,8 +1355,10 @@
       <c r="K31" s="1">
         <v>0.75718639833306223</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1318,8 +1392,10 @@
       <c r="K32" s="1">
         <v>0.69266852295693071</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -1353,8 +1429,10 @@
       <c r="K33" s="1">
         <v>0.78099650687006228</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -1388,8 +1466,10 @@
       <c r="K34" s="1">
         <v>0.76129975283755569</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -1423,8 +1503,10 @@
       <c r="K35" s="1">
         <v>0.77014120680256104</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
@@ -1458,8 +1540,10 @@
       <c r="K36" s="1">
         <v>0.77215505290505682</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -1493,8 +1577,10 @@
       <c r="K37" s="1">
         <v>0.77114812985380909</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>21</v>
       </c>
@@ -1502,7 +1588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>19</v>
       </c>
@@ -1533,8 +1619,17 @@
       <c r="K41" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -1568,8 +1663,20 @@
       <c r="K42" s="1">
         <v>0.92255148781433083</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M42" s="1">
+        <f>MIN(B42:K49)</f>
+        <v>0.72135852693187918</v>
+      </c>
+      <c r="N42" s="1">
+        <f>MAX(B42:K49)</f>
+        <v>0.93287487160864513</v>
+      </c>
+      <c r="O42">
+        <f>ABS(M42-N42)</f>
+        <v>0.21151634467676594</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>6</v>
       </c>
@@ -1603,8 +1710,10 @@
       <c r="K43" s="1">
         <v>0.80395625175287899</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1638,8 +1747,10 @@
       <c r="K44" s="1">
         <v>0.77191166192933314</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
@@ -1673,8 +1784,10 @@
       <c r="K45" s="1">
         <v>0.82567227108597252</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
@@ -1708,8 +1821,10 @@
       <c r="K46" s="1">
         <v>0.83994066324505612</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
@@ -1743,8 +1858,10 @@
       <c r="K47" s="1">
         <v>0.83287796926185331</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
@@ -1778,8 +1895,10 @@
       <c r="K48" s="1">
         <v>0.83273496506917544</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -1813,8 +1932,10 @@
       <c r="K49" s="1">
         <v>0.83280646716551421</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>14</v>
       </c>
@@ -1822,7 +1943,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>12</v>
       </c>
@@ -1853,8 +1974,17 @@
       <c r="K53" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M53" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -1888,8 +2018,20 @@
       <c r="K54" s="1">
         <v>0.8359042862056556</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M54" s="1">
+        <f>MIN(B54:K61)</f>
+        <v>0.78045190617034366</v>
+      </c>
+      <c r="N54" s="1">
+        <f>MAX(B54:K61)</f>
+        <v>0.86611097737823406</v>
+      </c>
+      <c r="O54">
+        <f>ABS(M54-N54)</f>
+        <v>8.5659071207890403E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>6</v>
       </c>
@@ -1923,8 +2065,10 @@
       <c r="K55" s="1">
         <v>0.78549343630932922</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>5</v>
       </c>
@@ -1958,8 +2102,10 @@
       <c r="K56" s="1">
         <v>0.79567159955620848</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
@@ -1993,8 +2139,10 @@
       <c r="K57" s="1">
         <v>0.80973103857313922</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>3</v>
       </c>
@@ -2028,8 +2176,10 @@
       <c r="K58" s="1">
         <v>0.80164850947432287</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>2</v>
       </c>
@@ -2063,8 +2213,10 @@
       <c r="K59" s="1">
         <v>0.80610693792986354</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>1</v>
       </c>
@@ -2098,8 +2250,10 @@
       <c r="K60" s="1">
         <v>0.80527261011759876</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -2133,6 +2287,8 @@
       <c r="K61" s="1">
         <v>0.80568977402373121</v>
       </c>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>